<commit_message>
finalTask debug code deleted
</commit_message>
<xml_diff>
--- a/datafile.xlsx
+++ b/datafile.xlsx
@@ -13,7 +13,151 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+  <si>
+    <t>Dates</t>
+  </si>
+  <si>
+    <t>Bases</t>
+  </si>
+  <si>
+    <t>Changes</t>
+  </si>
+  <si>
+    <t>Differs</t>
+  </si>
+  <si>
+    <t>Dates</t>
+  </si>
+  <si>
+    <t>Bases</t>
+  </si>
+  <si>
+    <t>Changes</t>
+  </si>
+  <si>
+    <t>Differs</t>
+  </si>
+  <si>
+    <t>Dates</t>
+  </si>
+  <si>
+    <t>Bases</t>
+  </si>
+  <si>
+    <t>Changes</t>
+  </si>
+  <si>
+    <t>Differs</t>
+  </si>
+  <si>
+    <t>Dates</t>
+  </si>
+  <si>
+    <t>Bases</t>
+  </si>
+  <si>
+    <t>Changes</t>
+  </si>
+  <si>
+    <t>Differs</t>
+  </si>
+  <si>
+    <t>Dates</t>
+  </si>
+  <si>
+    <t>Bases</t>
+  </si>
+  <si>
+    <t>Changes</t>
+  </si>
+  <si>
+    <t>Differs</t>
+  </si>
+  <si>
+    <t>Dates</t>
+  </si>
+  <si>
+    <t>Bases</t>
+  </si>
+  <si>
+    <t>Changes</t>
+  </si>
+  <si>
+    <t>Differs</t>
+  </si>
+  <si>
+    <t>Dates</t>
+  </si>
+  <si>
+    <t>Bases</t>
+  </si>
+  <si>
+    <t>Changes</t>
+  </si>
+  <si>
+    <t>Differs</t>
+  </si>
+  <si>
+    <t>Dates</t>
+  </si>
+  <si>
+    <t>Bases</t>
+  </si>
+  <si>
+    <t>Changes</t>
+  </si>
+  <si>
+    <t>Differs</t>
+  </si>
+  <si>
+    <t>Dates</t>
+  </si>
+  <si>
+    <t>Bases</t>
+  </si>
+  <si>
+    <t>Changes</t>
+  </si>
+  <si>
+    <t>Differs</t>
+  </si>
+  <si>
+    <t>Dates</t>
+  </si>
+  <si>
+    <t>Bases</t>
+  </si>
+  <si>
+    <t>Changes</t>
+  </si>
+  <si>
+    <t>Differs</t>
+  </si>
+  <si>
+    <t>Dates</t>
+  </si>
+  <si>
+    <t>Bases</t>
+  </si>
+  <si>
+    <t>Changes</t>
+  </si>
+  <si>
+    <t>Differs</t>
+  </si>
+  <si>
+    <t>Dates</t>
+  </si>
+  <si>
+    <t>Bases</t>
+  </si>
+  <si>
+    <t>Changes</t>
+  </si>
+  <si>
+    <t>Differs</t>
+  </si>
   <si>
     <t>Dates</t>
   </si>
@@ -93,7 +237,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -106,17 +250,41 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -137,16 +305,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2">

</xml_diff>